<commit_message>
SF analysis: 24H WD vs Control
</commit_message>
<xml_diff>
--- a/data/WD_PA 25 12 26_1_v2.xlsx
+++ b/data/WD_PA 25 12 26_1_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="32000" windowHeight="14720" activeTab="1"/>
+    <workbookView windowHeight="16560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="157">
   <si>
     <t>Column</t>
   </si>
@@ -339,7 +339,13 @@
     <t>RatID</t>
   </si>
   <si>
+    <t>Measurement1</t>
+  </si>
+  <si>
     <t>Treatment 2 /rat groups</t>
+  </si>
+  <si>
+    <t>Measurement3</t>
   </si>
   <si>
     <t>Hand 1.1</t>
@@ -1558,7 +1564,7 @@
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{5D5292B6-F0C4-A184-AD5C-7669409B0B0A}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{23979706-AC42-65F9-B665-776940C78DAB}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2526,7 +2532,7 @@
   <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.78125" defaultRowHeight="16.8"/>
@@ -2555,57 +2561,57 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" s="2">
         <v>354</v>
@@ -2617,7 +2623,7 @@
         <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I2" s="3">
         <v>2</v>
@@ -2643,7 +2649,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2">
         <v>333</v>
@@ -2655,7 +2661,7 @@
         <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>37</v>
@@ -2705,7 +2711,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B4" s="2">
         <v>397</v>
@@ -2717,7 +2723,7 @@
         <v>48</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>37</v>
@@ -2767,7 +2773,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B5" s="2">
         <v>412</v>
@@ -2779,7 +2785,7 @@
         <v>48</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>37</v>
@@ -2829,7 +2835,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B6" s="2">
         <v>311</v>
@@ -2841,7 +2847,7 @@
         <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>37</v>
@@ -2891,7 +2897,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B7" s="2">
         <v>321</v>
@@ -2903,7 +2909,7 @@
         <v>48</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>37</v>
@@ -2953,7 +2959,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B8" s="2">
         <v>342</v>
@@ -2965,7 +2971,7 @@
         <v>48</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>37</v>
@@ -3015,7 +3021,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B9" s="2">
         <v>362</v>
@@ -3027,7 +3033,7 @@
         <v>48</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>37</v>
@@ -3075,7 +3081,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B10" s="2">
         <v>376</v>
@@ -3087,16 +3093,16 @@
         <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I10" s="3">
         <v>2</v>
@@ -3134,7 +3140,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B11" s="2">
         <v>394</v>
@@ -3146,7 +3152,7 @@
         <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I11" s="3">
         <v>1</v>
@@ -3172,7 +3178,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B12" s="2">
         <v>415</v>
@@ -3184,16 +3190,16 @@
         <v>48</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I12" s="3">
         <v>2</v>
@@ -3234,7 +3240,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B13" s="2">
         <v>431</v>
@@ -3246,7 +3252,7 @@
         <v>48</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I13" s="3">
         <v>0</v>
@@ -3272,7 +3278,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B14" s="2">
         <v>474</v>
@@ -3284,16 +3290,16 @@
         <v>48</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I14" s="3">
         <v>4</v>
@@ -3334,7 +3340,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B15" s="2">
         <v>323</v>
@@ -3346,16 +3352,16 @@
         <v>48</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I15" s="3">
         <v>2</v>
@@ -3396,7 +3402,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B16" s="2">
         <v>199</v>
@@ -3408,16 +3414,16 @@
         <v>48</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I16" s="3">
         <v>2</v>
@@ -3458,7 +3464,7 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B17" s="2">
         <v>396</v>
@@ -3470,16 +3476,16 @@
         <v>48</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I17" s="3">
         <v>2</v>
@@ -3520,7 +3526,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B18" s="2">
         <v>388</v>
@@ -3538,10 +3544,10 @@
         <v>52</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I18" s="3">
         <v>0.5</v>
@@ -3582,7 +3588,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B19" s="2">
         <v>392</v>
@@ -3600,10 +3606,10 @@
         <v>52</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I19" s="3">
         <v>0.5</v>
@@ -3644,7 +3650,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B20" s="2">
         <v>381</v>
@@ -3662,10 +3668,10 @@
         <v>52</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I20" s="3">
         <v>-1</v>
@@ -3706,7 +3712,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B21" s="2">
         <v>286</v>
@@ -3724,10 +3730,10 @@
         <v>52</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I21" s="3">
         <v>0.5</v>
@@ -3768,7 +3774,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B22" s="2">
         <v>293</v>
@@ -3786,10 +3792,10 @@
         <v>52</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I22" s="3">
         <v>0</v>
@@ -3830,7 +3836,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B23" s="2">
         <v>309</v>
@@ -3848,10 +3854,10 @@
         <v>52</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I23" s="3">
         <v>0</v>
@@ -3892,7 +3898,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B24" s="2">
         <v>185</v>
@@ -3930,7 +3936,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C25" s="2">
         <v>202</v>
@@ -3945,10 +3951,10 @@
         <v>52</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I25" s="3">
         <v>0.5</v>
@@ -3989,7 +3995,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B26" s="2">
         <v>238</v>
@@ -4001,7 +4007,7 @@
         <v>48</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I26" s="3">
         <v>4</v>
@@ -4027,7 +4033,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B27" s="2">
         <v>246</v>
@@ -4045,10 +4051,10 @@
         <v>39</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I27" s="3">
         <v>0</v>
@@ -4089,7 +4095,7 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B28" s="2">
         <v>181</v>
@@ -4101,7 +4107,7 @@
         <v>48</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I28" s="3">
         <v>-0.5</v>
@@ -4127,7 +4133,7 @@
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B29" s="2">
         <v>184</v>
@@ -4139,7 +4145,7 @@
         <v>48</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I29" s="3">
         <v>-3.5</v>
@@ -4163,7 +4169,7 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B30" s="2">
         <v>218</v>
@@ -4181,10 +4187,10 @@
         <v>39</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I30" s="3">
         <v>0</v>
@@ -4225,7 +4231,7 @@
     </row>
     <row r="31" spans="1:20">
       <c r="A31" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B31" s="2">
         <v>235</v>
@@ -4243,10 +4249,10 @@
         <v>39</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I31" s="3">
         <v>1</v>
@@ -4287,7 +4293,7 @@
     </row>
     <row r="32" spans="1:20">
       <c r="A32" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B32" s="2">
         <v>250</v>
@@ -4305,10 +4311,10 @@
         <v>39</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I32" s="3">
         <v>0</v>
@@ -4349,7 +4355,7 @@
     </row>
     <row r="33" spans="1:20">
       <c r="A33" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B33" s="2">
         <v>147</v>
@@ -4361,7 +4367,7 @@
         <v>48</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>39</v>
@@ -4411,7 +4417,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B34" s="2">
         <v>164</v>
@@ -4423,7 +4429,7 @@
         <v>48</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>39</v>
@@ -4473,7 +4479,7 @@
     </row>
     <row r="35" spans="1:20">
       <c r="A35" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B35" s="2">
         <v>160</v>
@@ -4485,7 +4491,7 @@
         <v>48</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>39</v>
@@ -4535,7 +4541,7 @@
     </row>
     <row r="36" spans="1:20">
       <c r="A36" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B36" s="2">
         <v>202</v>
@@ -4547,7 +4553,7 @@
         <v>48</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>39</v>
@@ -4597,7 +4603,7 @@
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B37" s="2">
         <v>201</v>
@@ -4609,7 +4615,7 @@
         <v>48</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>39</v>
@@ -4659,7 +4665,7 @@
     </row>
     <row r="38" spans="1:20">
       <c r="A38" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B38" s="2">
         <v>209</v>
@@ -4671,7 +4677,7 @@
         <v>48</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>39</v>
@@ -4721,7 +4727,7 @@
     </row>
     <row r="39" spans="1:20">
       <c r="A39" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B39" s="2">
         <v>205</v>
@@ -4733,7 +4739,7 @@
         <v>48</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I39" s="3">
         <v>1.5</v>
@@ -4759,7 +4765,7 @@
     </row>
     <row r="40" spans="1:20">
       <c r="A40" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B40" s="2">
         <v>207</v>
@@ -4771,7 +4777,7 @@
         <v>48</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>39</v>
@@ -4821,7 +4827,7 @@
     </row>
     <row r="41" spans="1:20">
       <c r="A41" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B41" s="2">
         <v>242</v>
@@ -4833,7 +4839,7 @@
         <v>48</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I41" s="3">
         <v>2.5</v>
@@ -4859,7 +4865,7 @@
     </row>
     <row r="42" spans="1:20">
       <c r="A42" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B42" s="2">
         <v>288</v>
@@ -4871,7 +4877,7 @@
         <v>48</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>52</v>
@@ -4921,7 +4927,7 @@
     </row>
     <row r="43" spans="1:20">
       <c r="A43" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B43" s="2">
         <v>178</v>
@@ -4933,7 +4939,7 @@
         <v>48</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>52</v>
@@ -4983,7 +4989,7 @@
     </row>
     <row r="44" spans="1:20">
       <c r="A44" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B44" s="2">
         <v>149</v>
@@ -4995,7 +5001,7 @@
         <v>48</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>52</v>
@@ -5045,7 +5051,7 @@
     </row>
     <row r="45" spans="1:20">
       <c r="A45" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B45" s="2">
         <v>151</v>
@@ -5057,7 +5063,7 @@
         <v>48</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I45" s="3">
         <v>1</v>
@@ -5083,7 +5089,7 @@
     </row>
     <row r="46" spans="1:20">
       <c r="A46" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B46" s="5">
         <v>193</v>
@@ -5095,7 +5101,7 @@
         <v>48</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>52</v>
@@ -5145,7 +5151,7 @@
     </row>
     <row r="47" spans="1:20">
       <c r="A47" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B47" s="5">
         <v>209</v>
@@ -5157,7 +5163,7 @@
         <v>48</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>52</v>
@@ -5207,7 +5213,7 @@
     </row>
     <row r="48" spans="1:20">
       <c r="A48" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B48" s="5">
         <v>203</v>
@@ -5219,7 +5225,7 @@
         <v>48</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
@@ -5248,7 +5254,7 @@
     </row>
     <row r="49" spans="1:20">
       <c r="A49" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B49" s="5">
         <v>177</v>
@@ -5260,7 +5266,7 @@
         <v>48</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>52</v>
@@ -5310,7 +5316,7 @@
     </row>
     <row r="50" spans="1:20">
       <c r="A50" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B50" s="5">
         <v>160</v>
@@ -5322,7 +5328,7 @@
         <v>48</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>52</v>
@@ -5370,7 +5376,7 @@
     </row>
     <row r="51" spans="1:20">
       <c r="A51" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B51" s="5">
         <v>193</v>
@@ -5382,7 +5388,7 @@
         <v>48</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -5411,7 +5417,7 @@
     </row>
     <row r="52" spans="1:20">
       <c r="A52" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B52" s="5">
         <v>220</v>
@@ -5423,16 +5429,16 @@
         <v>48</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I52" s="3">
         <v>5.5</v>
@@ -5473,7 +5479,7 @@
     </row>
     <row r="53" spans="1:20">
       <c r="A53" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B53" s="5">
         <v>269</v>
@@ -5485,7 +5491,7 @@
         <v>48</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -5514,7 +5520,7 @@
     </row>
     <row r="54" spans="1:20">
       <c r="A54" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B54" s="5">
         <v>251</v>
@@ -5526,16 +5532,16 @@
         <v>48</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I54" s="3">
         <v>2.5</v>
@@ -5576,7 +5582,7 @@
     </row>
     <row r="55" spans="1:20">
       <c r="A55" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B55" s="5">
         <v>201</v>
@@ -5588,16 +5594,16 @@
         <v>48</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I55" s="3">
         <v>2</v>
@@ -5638,7 +5644,7 @@
     </row>
     <row r="56" spans="1:20">
       <c r="A56" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B56" s="5">
         <v>253</v>
@@ -5650,16 +5656,16 @@
         <v>48</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I56" s="3">
         <v>2.5</v>

</xml_diff>